<commit_message>
removed atmospheric data columns from configuration Excel spreadsheet
</commit_message>
<xml_diff>
--- a/Example/configuration_example_project.xlsx
+++ b/Example/configuration_example_project.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aearntsen/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\site_suitability_tool\Example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5688AA31-8D1F-6148-81C3-19AFC5D5E76A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1CB8C67-BE27-46F7-A8CF-BB0E731B2D5A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-91780" yWindow="5400" windowWidth="22800" windowHeight="17080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Configuration_template" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Lable" sheetId="3" r:id="rId3"/>
     <sheet name="RSD_Models" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterate="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="307">
   <si>
     <t>Timestamp</t>
   </si>
@@ -1571,28 +1571,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M125"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="46.1640625" customWidth="1"/>
+    <col min="1" max="1" width="46.1796875" customWidth="1"/>
     <col min="2" max="2" width="20" customWidth="1"/>
-    <col min="3" max="3" width="6.5" customWidth="1"/>
-    <col min="4" max="4" width="66.1640625" customWidth="1"/>
-    <col min="5" max="5" width="16.83203125" customWidth="1"/>
-    <col min="6" max="6" width="18.83203125" customWidth="1"/>
-    <col min="7" max="7" width="3.5" customWidth="1"/>
-    <col min="8" max="8" width="46.5" customWidth="1"/>
-    <col min="9" max="9" width="9.33203125" customWidth="1"/>
-    <col min="10" max="10" width="30.6640625" customWidth="1"/>
-    <col min="11" max="11" width="3.5" customWidth="1"/>
-    <col min="12" max="12" width="32.6640625" customWidth="1"/>
-    <col min="13" max="13" width="11.6640625" customWidth="1"/>
+    <col min="3" max="3" width="6.453125" customWidth="1"/>
+    <col min="4" max="4" width="66.1796875" customWidth="1"/>
+    <col min="5" max="5" width="16.81640625" customWidth="1"/>
+    <col min="6" max="6" width="18.81640625" customWidth="1"/>
+    <col min="7" max="7" width="3.453125" customWidth="1"/>
+    <col min="8" max="8" width="46.453125" customWidth="1"/>
+    <col min="9" max="9" width="9.36328125" customWidth="1"/>
+    <col min="10" max="10" width="30.6328125" customWidth="1"/>
+    <col min="11" max="11" width="3.453125" customWidth="1"/>
+    <col min="12" max="12" width="32.6328125" customWidth="1"/>
+    <col min="13" max="13" width="11.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>65</v>
       </c>
@@ -1627,7 +1627,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="E2" t="s">
         <v>23</v>
       </c>
@@ -1637,7 +1637,7 @@
       <c r="L2" s="1"/>
       <c r="M2" s="8"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -1663,7 +1663,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>306</v>
       </c>
@@ -1686,7 +1686,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>158</v>
       </c>
@@ -1706,7 +1706,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>159</v>
       </c>
@@ -1726,7 +1726,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>261</v>
       </c>
@@ -1746,7 +1746,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>160</v>
       </c>
@@ -1766,7 +1766,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>301</v>
       </c>
@@ -1786,7 +1786,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>161</v>
       </c>
@@ -1806,7 +1806,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>257</v>
       </c>
@@ -1820,7 +1820,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>162</v>
       </c>
@@ -1840,7 +1840,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>163</v>
       </c>
@@ -1854,7 +1854,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>259</v>
       </c>
@@ -1868,7 +1868,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>164</v>
       </c>
@@ -1882,7 +1882,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>165</v>
       </c>
@@ -1896,7 +1896,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>260</v>
       </c>
@@ -1907,7 +1907,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>166</v>
       </c>
@@ -1918,7 +1918,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>167</v>
       </c>
@@ -1929,7 +1929,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>262</v>
       </c>
@@ -1940,7 +1940,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>168</v>
       </c>
@@ -1948,7 +1948,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>169</v>
       </c>
@@ -1959,7 +1959,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>263</v>
       </c>
@@ -1970,7 +1970,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>170</v>
       </c>
@@ -1984,7 +1984,7 @@
         <v>42.4</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>171</v>
       </c>
@@ -1998,7 +1998,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>264</v>
       </c>
@@ -2006,7 +2006,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>300</v>
       </c>
@@ -2014,86 +2014,77 @@
         <v>298</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>181</v>
       </c>
-      <c r="B38" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>182</v>
       </c>
-      <c r="B39" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>183</v>
       </c>
-      <c r="B40" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>185</v>
       </c>
@@ -2101,7 +2092,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>186</v>
       </c>
@@ -2109,22 +2100,22 @@
         <v>286</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>190</v>
       </c>
@@ -2132,27 +2123,27 @@
         <v>291</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>195</v>
       </c>
@@ -2160,7 +2151,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>196</v>
       </c>
@@ -2168,22 +2159,22 @@
         <v>287</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>200</v>
       </c>
@@ -2191,7 +2182,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>201</v>
       </c>
@@ -2199,47 +2190,47 @@
         <v>290</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>210</v>
       </c>
@@ -2247,7 +2238,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>211</v>
       </c>
@@ -2255,147 +2246,147 @@
         <v>288</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>240</v>
       </c>
@@ -2403,27 +2394,27 @@
         <v>292</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>245</v>
       </c>
@@ -2431,12 +2422,12 @@
         <v>146</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>247</v>
       </c>
@@ -2444,7 +2435,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>248</v>
       </c>
@@ -2452,12 +2443,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>250</v>
       </c>
@@ -2465,37 +2456,37 @@
         <v>152</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
         <v>265</v>
       </c>
@@ -2503,12 +2494,12 @@
         <v>145</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
         <v>267</v>
       </c>
@@ -2516,7 +2507,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
         <v>268</v>
       </c>
@@ -2524,12 +2515,12 @@
         <v>62</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
         <v>270</v>
       </c>
@@ -2537,32 +2528,32 @@
         <v>151</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
         <v>276</v>
       </c>
@@ -2726,19 +2717,19 @@
       <selection activeCell="L28" sqref="L28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.83203125" customWidth="1"/>
-    <col min="2" max="2" width="16.6640625" customWidth="1"/>
-    <col min="3" max="3" width="18.5" customWidth="1"/>
-    <col min="4" max="4" width="18.83203125" customWidth="1"/>
-    <col min="11" max="11" width="21.5" customWidth="1"/>
-    <col min="12" max="12" width="20.5" customWidth="1"/>
+    <col min="1" max="1" width="14.81640625" customWidth="1"/>
+    <col min="2" max="2" width="16.6328125" customWidth="1"/>
+    <col min="3" max="3" width="18.453125" customWidth="1"/>
+    <col min="4" max="4" width="18.81640625" customWidth="1"/>
+    <col min="11" max="11" width="21.453125" customWidth="1"/>
+    <col min="12" max="12" width="20.453125" customWidth="1"/>
     <col min="13" max="13" width="49" customWidth="1"/>
-    <col min="14" max="14" width="14.6640625" customWidth="1"/>
+    <col min="14" max="14" width="14.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>26</v>
       </c>
@@ -2795,7 +2786,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>117</v>
       </c>
@@ -2848,7 +2839,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>67</v>
       </c>
@@ -2901,7 +2892,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>68</v>
       </c>
@@ -2933,7 +2924,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>69</v>
       </c>
@@ -2953,7 +2944,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>70</v>
       </c>
@@ -2970,7 +2961,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>71</v>
       </c>
@@ -2981,7 +2972,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>72</v>
       </c>
@@ -2989,7 +2980,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>73</v>
       </c>
@@ -2997,223 +2988,227 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>116</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;1#&amp;"Arial"&amp;11&amp;K404040Restricted</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -3225,262 +3220,262 @@
       <selection activeCell="A52" sqref="A52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.5" customWidth="1"/>
+    <col min="1" max="1" width="25.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>306</v>
       </c>
@@ -3505,62 +3500,62 @@
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.1640625" customWidth="1"/>
+    <col min="1" max="1" width="14.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>280</v>
       </c>

</xml_diff>

<commit_message>
moved methodolgoy to sub-sub package
</commit_message>
<xml_diff>
--- a/Example/configuration_example_project.xlsx
+++ b/Example/configuration_example_project.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\site_suitability_tool\Example\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\drc\gits\TACT\Example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1CB8C67-BE27-46F7-A8CF-BB0E731B2D5A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4D93BA4-C4D5-49A3-9A99-ADD0231B4E14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28095" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Configuration_template" sheetId="1" r:id="rId1"/>
@@ -65,12 +65,6 @@
     <t>corrWS_RSD_WS</t>
   </si>
   <si>
-    <t>corrTI_RSD_TI</t>
-  </si>
-  <si>
-    <t>corrTI_RSD_WS</t>
-  </si>
-  <si>
     <t>WindCube v1</t>
   </si>
   <si>
@@ -143,9 +137,6 @@
     <t>Anemometer 2 Class:</t>
   </si>
   <si>
-    <t>RSD TI Correction Method Applied:</t>
-  </si>
-  <si>
     <t>Does anemometer mounting meet Measnet/IEC Standards?</t>
   </si>
   <si>
@@ -957,6 +948,15 @@
   </si>
   <si>
     <t>Hour</t>
+  </si>
+  <si>
+    <t>RSD TI Adjustment Method Applied:</t>
+  </si>
+  <si>
+    <t>adjTI_RSD_TI</t>
+  </si>
+  <si>
+    <t>adjTI_RSD_WS</t>
   </si>
 </sst>
 </file>
@@ -1571,73 +1571,73 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="46.1796875" customWidth="1"/>
+    <col min="1" max="1" width="46.140625" customWidth="1"/>
     <col min="2" max="2" width="20" customWidth="1"/>
-    <col min="3" max="3" width="6.453125" customWidth="1"/>
-    <col min="4" max="4" width="66.1796875" customWidth="1"/>
-    <col min="5" max="5" width="16.81640625" customWidth="1"/>
-    <col min="6" max="6" width="18.81640625" customWidth="1"/>
-    <col min="7" max="7" width="3.453125" customWidth="1"/>
-    <col min="8" max="8" width="46.453125" customWidth="1"/>
-    <col min="9" max="9" width="9.36328125" customWidth="1"/>
-    <col min="10" max="10" width="30.6328125" customWidth="1"/>
-    <col min="11" max="11" width="3.453125" customWidth="1"/>
-    <col min="12" max="12" width="32.6328125" customWidth="1"/>
-    <col min="13" max="13" width="11.6328125" customWidth="1"/>
+    <col min="3" max="3" width="6.42578125" customWidth="1"/>
+    <col min="4" max="4" width="66.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" customWidth="1"/>
+    <col min="6" max="6" width="18.85546875" customWidth="1"/>
+    <col min="7" max="7" width="3.42578125" customWidth="1"/>
+    <col min="8" max="8" width="46.42578125" customWidth="1"/>
+    <col min="9" max="9" width="9.42578125" customWidth="1"/>
+    <col min="10" max="10" width="30.5703125" customWidth="1"/>
+    <col min="11" max="11" width="3.42578125" customWidth="1"/>
+    <col min="12" max="12" width="32.5703125" customWidth="1"/>
+    <col min="13" max="13" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="I1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="J1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="L1" s="6" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="M1" s="7" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="L2" s="1"/>
       <c r="M2" s="8"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -1645,917 +1645,917 @@
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E3" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="H3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="I3" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="M3" s="9" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="B4" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="D4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="I4" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="J4" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B5" t="s">
         <v>3</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="E5">
         <v>55</v>
       </c>
       <c r="H5" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="I5" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B6" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E6" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="H6" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="I6" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="B7" t="s">
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E7">
         <v>60</v>
       </c>
       <c r="H7" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="I7" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B8" t="s">
         <v>5</v>
       </c>
       <c r="D8" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" t="s">
+        <v>124</v>
+      </c>
+      <c r="H8" t="s">
+        <v>51</v>
+      </c>
+      <c r="I8" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>298</v>
+      </c>
+      <c r="B9" t="s">
+        <v>296</v>
+      </c>
+      <c r="D9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" t="s">
+        <v>40</v>
+      </c>
+      <c r="H9" t="s">
+        <v>299</v>
+      </c>
+      <c r="I9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>158</v>
+      </c>
+      <c r="B10" t="s">
+        <v>60</v>
+      </c>
+      <c r="D10" t="s">
         <v>30</v>
       </c>
-      <c r="E8" t="s">
-        <v>127</v>
-      </c>
-      <c r="H8" t="s">
-        <v>54</v>
-      </c>
-      <c r="I8" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>301</v>
-      </c>
-      <c r="B9" t="s">
-        <v>299</v>
-      </c>
-      <c r="D9" t="s">
-        <v>31</v>
-      </c>
-      <c r="E9" t="s">
-        <v>43</v>
-      </c>
-      <c r="H9" t="s">
-        <v>302</v>
-      </c>
-      <c r="I9" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>161</v>
-      </c>
-      <c r="B10" t="s">
-        <v>63</v>
-      </c>
-      <c r="D10" t="s">
-        <v>32</v>
-      </c>
       <c r="E10" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="H10" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="I10" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="B11" t="s">
         <v>2</v>
       </c>
       <c r="D11" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E11">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B12" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="D12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E12">
         <v>1</v>
       </c>
       <c r="H12" s="10" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="I12" s="11" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B13" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D13" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E13" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="B14" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D14" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="E14">
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B15" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D15" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="E15">
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B16" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D16" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="E16">
         <v>65</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="B17" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="D17" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D18" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="E18">
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D19" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="E19">
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="D20" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="E20">
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="D21" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="E22">
         <v>45</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="E23">
         <v>180</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B24" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="E24">
         <v>42.4</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B25" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="E25">
         <v>55</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="B26" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="B27" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A38" t="s">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A39" t="s">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A40" t="s">
+      <c r="B42" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A41" t="s">
+      <c r="B43" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A42" t="s">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>185</v>
       </c>
-      <c r="B42" t="s">
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>187</v>
+      </c>
+      <c r="B47" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>192</v>
+      </c>
+      <c r="B52" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A43" t="s">
-        <v>186</v>
-      </c>
-      <c r="B43" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A44" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A45" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A46" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A47" t="s">
-        <v>190</v>
-      </c>
-      <c r="B47" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A48" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A49" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A50" t="s">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A51" t="s">
+      <c r="B53" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A52" t="s">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
         <v>195</v>
       </c>
-      <c r="B52" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A53" t="s">
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
         <v>196</v>
       </c>
-      <c r="B53" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A54" t="s">
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
         <v>197</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A55" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A56" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A57" t="s">
-        <v>200</v>
       </c>
       <c r="B57" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
+        <v>198</v>
+      </c>
+      <c r="B58" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
         <v>201</v>
       </c>
-      <c r="B58" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A59" t="s">
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A60" t="s">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A61" t="s">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A62" t="s">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A63" t="s">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A64" t="s">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A65" t="s">
+      <c r="B67" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A66" t="s">
+      <c r="B68" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A67" t="s">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
         <v>210</v>
       </c>
-      <c r="B67" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A68" t="s">
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
         <v>211</v>
       </c>
-      <c r="B68" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A69" t="s">
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A70" t="s">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A71" t="s">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A72" t="s">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A73" t="s">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A74" t="s">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A75" t="s">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A76" t="s">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A77" t="s">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A78" t="s">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A79" t="s">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A80" t="s">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A81" t="s">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A82" t="s">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A83" t="s">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A84" t="s">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A85" t="s">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A86" t="s">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A87" t="s">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A88" t="s">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A89" t="s">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A90" t="s">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A91" t="s">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A92" t="s">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A93" t="s">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A94" t="s">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A95" t="s">
+      <c r="B97" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A96" t="s">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A97" t="s">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
         <v>240</v>
       </c>
-      <c r="B97" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A98" t="s">
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A99" t="s">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A100" t="s">
+      <c r="B102" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A101" t="s">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A102" t="s">
+      <c r="B104" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
         <v>245</v>
-      </c>
-      <c r="B102" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A103" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A104" t="s">
-        <v>247</v>
-      </c>
-      <c r="B104" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A105" t="s">
-        <v>248</v>
       </c>
       <c r="B105" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>247</v>
+      </c>
+      <c r="B107" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A107" t="s">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
         <v>250</v>
       </c>
-      <c r="B107" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A108" t="s">
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A109" t="s">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A110" t="s">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A111" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A112" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A113" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
+        <v>262</v>
+      </c>
+      <c r="B114" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>264</v>
+      </c>
+      <c r="B116" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
         <v>265</v>
       </c>
-      <c r="B114" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A115" t="s">
+      <c r="B117" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A116" t="s">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
         <v>267</v>
       </c>
-      <c r="B116" t="s">
+      <c r="B119" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A117" t="s">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
         <v>268</v>
       </c>
-      <c r="B117" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A118" t="s">
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A119" t="s">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
         <v>270</v>
       </c>
-      <c r="B119" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A120" t="s">
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A121" t="s">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A122" t="s">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
         <v>273</v>
-      </c>
-    </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A123" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A124" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A125" t="s">
-        <v>276</v>
       </c>
     </row>
   </sheetData>
@@ -2713,94 +2713,94 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:S52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L28" sqref="L28"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.81640625" customWidth="1"/>
-    <col min="2" max="2" width="16.6328125" customWidth="1"/>
-    <col min="3" max="3" width="18.453125" customWidth="1"/>
-    <col min="4" max="4" width="18.81640625" customWidth="1"/>
-    <col min="11" max="11" width="21.453125" customWidth="1"/>
-    <col min="12" max="12" width="20.453125" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" customWidth="1"/>
+    <col min="4" max="4" width="18.85546875" customWidth="1"/>
+    <col min="11" max="11" width="21.42578125" customWidth="1"/>
+    <col min="12" max="12" width="20.42578125" customWidth="1"/>
     <col min="13" max="13" width="49" customWidth="1"/>
-    <col min="14" max="14" width="14.6328125" customWidth="1"/>
+    <col min="14" max="14" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C1" s="4"/>
       <c r="D1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="K1" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="L1" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="M1" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B2" t="s">
         <v>34</v>
       </c>
-      <c r="K1" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>117</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
+        <v>115</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" t="s">
         <v>37</v>
-      </c>
-      <c r="D2" t="s">
-        <v>118</v>
-      </c>
-      <c r="F2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" t="s">
-        <v>40</v>
       </c>
       <c r="H2">
         <v>1</v>
@@ -2812,48 +2812,48 @@
         <v>1</v>
       </c>
       <c r="K2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="L2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="M2" t="s">
+        <v>120</v>
+      </c>
+      <c r="N2" t="s">
+        <v>120</v>
+      </c>
+      <c r="O2" t="s">
+        <v>121</v>
+      </c>
+      <c r="P2" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>122</v>
+      </c>
+      <c r="R2" t="s">
+        <v>122</v>
+      </c>
+      <c r="S2" t="s">
         <v>123</v>
       </c>
-      <c r="N2" t="s">
-        <v>123</v>
-      </c>
-      <c r="O2" t="s">
-        <v>124</v>
-      </c>
-      <c r="P2" t="s">
-        <v>123</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>125</v>
-      </c>
-      <c r="R2" t="s">
-        <v>125</v>
-      </c>
-      <c r="S2" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" t="s">
+        <v>117</v>
+      </c>
+      <c r="F3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" t="s">
         <v>38</v>
-      </c>
-      <c r="D3" t="s">
-        <v>120</v>
-      </c>
-      <c r="F3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" t="s">
-        <v>41</v>
       </c>
       <c r="H3">
         <v>2</v>
@@ -2865,342 +2865,342 @@
         <v>2</v>
       </c>
       <c r="K3" t="s">
+        <v>17</v>
+      </c>
+      <c r="L3" t="s">
+        <v>56</v>
+      </c>
+      <c r="M3" t="s">
+        <v>56</v>
+      </c>
+      <c r="N3" t="s">
+        <v>56</v>
+      </c>
+      <c r="O3" t="s">
+        <v>56</v>
+      </c>
+      <c r="P3" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>56</v>
+      </c>
+      <c r="R3" t="s">
+        <v>56</v>
+      </c>
+      <c r="S3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" t="s">
+        <v>118</v>
+      </c>
+      <c r="F4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" t="s">
+        <v>39</v>
+      </c>
+      <c r="H4" t="s">
+        <v>42</v>
+      </c>
+      <c r="I4" t="s">
+        <v>42</v>
+      </c>
+      <c r="J4" t="s">
+        <v>42</v>
+      </c>
+      <c r="K4" t="s">
+        <v>18</v>
+      </c>
+      <c r="M4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" t="s">
+        <v>116</v>
+      </c>
+      <c r="F5" t="s">
         <v>19</v>
       </c>
-      <c r="L3" t="s">
-        <v>59</v>
-      </c>
-      <c r="M3" t="s">
-        <v>59</v>
-      </c>
-      <c r="N3" t="s">
-        <v>59</v>
-      </c>
-      <c r="O3" t="s">
-        <v>59</v>
-      </c>
-      <c r="P3" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>59</v>
-      </c>
-      <c r="R3" t="s">
-        <v>59</v>
-      </c>
-      <c r="S3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+      <c r="G5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>67</v>
+      </c>
+      <c r="D6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" t="s">
+        <v>41</v>
+      </c>
+      <c r="K6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>68</v>
       </c>
-      <c r="B4" t="s">
-        <v>39</v>
-      </c>
-      <c r="D4" t="s">
-        <v>121</v>
-      </c>
-      <c r="F4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" t="s">
+      <c r="F7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" t="s">
         <v>42</v>
       </c>
-      <c r="H4" t="s">
-        <v>45</v>
-      </c>
-      <c r="I4" t="s">
-        <v>45</v>
-      </c>
-      <c r="J4" t="s">
-        <v>45</v>
-      </c>
-      <c r="K4" t="s">
-        <v>20</v>
-      </c>
-      <c r="M4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>69</v>
       </c>
-      <c r="B5" t="s">
-        <v>47</v>
-      </c>
-      <c r="D5" t="s">
-        <v>119</v>
-      </c>
-      <c r="F5" t="s">
-        <v>21</v>
-      </c>
-      <c r="G5" t="s">
-        <v>43</v>
-      </c>
-      <c r="K5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+      <c r="F8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>70</v>
       </c>
-      <c r="D6" t="s">
-        <v>45</v>
-      </c>
-      <c r="F6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G6" t="s">
-        <v>44</v>
-      </c>
-      <c r="K6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+      <c r="F9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>71</v>
       </c>
-      <c r="F7" t="s">
-        <v>15</v>
-      </c>
-      <c r="G7" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>72</v>
       </c>
-      <c r="F8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>73</v>
       </c>
-      <c r="F9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A38" t="s">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A39" t="s">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A40" t="s">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A41" t="s">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A42" t="s">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A43" t="s">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A44" t="s">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A45" t="s">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A46" t="s">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A47" t="s">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A48" t="s">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A49" t="s">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
         <v>113</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A50" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A51" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A52" t="s">
-        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -3216,268 +3216,268 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:A51"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="A52" sqref="A52"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="A53" sqref="A53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.453125" customWidth="1"/>
+    <col min="1" max="1" width="25.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A38" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A39" t="s">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A40" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A41" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A42" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A43" t="s">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A44" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A45" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.35">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
         <v>303</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A49" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A50" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A51" t="s">
-        <v>306</v>
       </c>
     </row>
   </sheetData>
@@ -3496,68 +3496,66 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:A11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.1796875" customWidth="1"/>
+    <col min="1" max="1" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>277</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>280</v>
       </c>
     </row>
   </sheetData>

</xml_diff>